<commit_message>
correction and print result
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\playground\Dyson_Sphere_Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pengcheng/playground/Dyson_Sphere_Program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C3C95-26F8-418D-8759-9F57314EE1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E587F11-C532-C043-9D75-14D063D84D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="83" windowWidth="15390" windowHeight="10552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="660" windowWidth="15400" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>制造</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>白糖</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>生产类型 / Production type</t>
   </si>
   <si>
@@ -154,6 +150,10 @@
   </si>
   <si>
     <t>速度（倍率） /  Speed (ratio)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电磁涡轮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -161,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,26 +482,26 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -509,27 +509,21 @@
         <v>0.75</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -537,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -545,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -553,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -561,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -569,7 +563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -577,7 +571,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -585,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -593,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -601,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -609,7 +603,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -617,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -625,7 +619,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -633,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -641,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -649,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -657,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -665,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -673,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -681,7 +675,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -689,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -697,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -705,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -713,7 +707,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>25</v>
       </c>

</xml_diff>